<commit_message>
added mysql not implemented
</commit_message>
<xml_diff>
--- a/to_summarize.xlsx
+++ b/to_summarize.xlsx
@@ -586,8 +586,8 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Summarize the following text in 3 sentences, and include 1 direct quote from the content that encapsulates what it is all about: 
-134.71445655822754</t>
+          <t>Please rewrite this in the style of Jason Fladlien:
+185.74622321128845</t>
         </is>
       </c>
     </row>
@@ -690,8 +690,8 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Summarize the following text in 3 sentences, and include 1 direct quote from the content that encapsulates what it is all about: 
-44.3434374332428</t>
+          <t>Please rewrite this in the style of Jason Fladlien:
+87.75262379646301</t>
         </is>
       </c>
     </row>
@@ -785,8 +785,8 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Summarize the following text in 3 sentences, and include 1 direct quote from the content that encapsulates what it is all about: 
-43.50903129577637</t>
+          <t>Please rewrite this in the style of Jason Fladlien:
+61.15979361534119</t>
         </is>
       </c>
     </row>
@@ -883,8 +883,8 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Summarize the following text in 3 sentences, and include 1 direct quote from the content that encapsulates what it is all about: 
-71.33363103866577</t>
+          <t>Please rewrite this in the style of Jason Fladlien:
+141.45266103744507</t>
         </is>
       </c>
     </row>
@@ -984,8 +984,8 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Summarize the following text in 3 sentences, and include 1 direct quote from the content that encapsulates what it is all about: 
-92.65366101264954</t>
+          <t>Please rewrite this in the style of Jason Fladlien:
+154.113951921463</t>
         </is>
       </c>
     </row>
@@ -1092,8 +1092,8 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Summarize the following text in 3 sentences, and include 1 direct quote from the content that encapsulates what it is all about: 
-70.70129156112671</t>
+          <t>Please rewrite this in the style of Jason Fladlien:
+143.74763584136963</t>
         </is>
       </c>
     </row>
@@ -1200,8 +1200,8 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Summarize the following text in 3 sentences, and include 1 direct quote from the content that encapsulates what it is all about: 
-46.09036588668823</t>
+          <t>Please rewrite this in the style of Jason Fladlien:
+77.22561883926392</t>
         </is>
       </c>
     </row>
@@ -1303,8 +1303,8 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Summarize the following text in 3 sentences, and include 1 direct quote from the content that encapsulates what it is all about: 
-41.89961004257202</t>
+          <t>Please rewrite this in the style of Jason Fladlien:
+68.87961220741272</t>
         </is>
       </c>
     </row>
@@ -1450,8 +1450,8 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Summarize the following text in 3 sentences, and include 1 direct quote from the content that encapsulates what it is all about: 
-184.78552889823914</t>
+          <t>Please rewrite this in the style of Jason Fladlien:
+161.40382480621338</t>
         </is>
       </c>
     </row>

</xml_diff>